<commit_message>
fix: trainee progress table
</commit_message>
<xml_diff>
--- a/TemporaryFileStorage/CourseList.xlsx
+++ b/TemporaryFileStorage/CourseList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavita.thomas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2019FFF2-E097-41C0-9B40-B8D8C37155C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB9BD120-701F-43AD-B8A2-7F2E695553D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{D88FFFD8-F634-4251-BFDF-C816D12817C9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="306">
   <si>
     <r>
       <t>ILP E-Learning Curriculum</t>
@@ -547,16 +547,10 @@
     <t> </t>
   </si>
   <si>
-    <t>plk,mnbvcsghjkllllllllmnbv</t>
-  </si>
-  <si>
     <t>Be Liked and Respected in the Workplace</t>
   </si>
   <si>
     <t>23m 36s</t>
-  </si>
-  <si>
-    <t>test2</t>
   </si>
   <si>
     <t>Building a Win-win Relationship with Your Manager</t>
@@ -1402,7 +1396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1571,6 +1565,39 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1580,39 +1607,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1622,7 +1616,6 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1970,15 +1963,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
     </row>
     <row r="2" spans="1:7" ht="15">
       <c r="A2" s="7" t="s">
@@ -2004,11 +1997,11 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2021,9 +2014,9 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="91"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2036,9 +2029,9 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A5" s="91"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
@@ -2053,9 +2046,9 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="91"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2070,9 +2063,9 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="94"/>
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
@@ -2100,13 +2093,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="86" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="9">
         <v>44806</v>
       </c>
-      <c r="C9" s="92"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2121,9 +2114,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="25.5">
-      <c r="A10" s="91"/>
-      <c r="B10" s="92"/>
-      <c r="C10" s="93"/>
+      <c r="A10" s="87"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2138,9 +2131,9 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="91"/>
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2155,9 +2148,9 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="91"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="44"/>
-      <c r="C12" s="93"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2172,9 +2165,9 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="94"/>
+      <c r="A13" s="88"/>
       <c r="B13" s="45"/>
-      <c r="C13" s="95"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2202,13 +2195,13 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="86" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="9">
         <v>44807</v>
       </c>
-      <c r="C15" s="92"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2223,9 +2216,9 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="91"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="93"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
@@ -2240,9 +2233,9 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="91"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
@@ -2257,9 +2250,9 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="91"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="90"/>
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2274,9 +2267,9 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="94"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="95"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2302,11 +2295,11 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
@@ -2321,9 +2314,9 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="91"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="93"/>
+      <c r="A22" s="87"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
@@ -2338,9 +2331,9 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="91"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="93"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2353,9 +2346,9 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="91"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="93"/>
+      <c r="A24" s="87"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2368,9 +2361,9 @@
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="94"/>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
       <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
@@ -2396,11 +2389,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
       <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
@@ -2415,9 +2408,9 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="91"/>
-      <c r="B28" s="93"/>
-      <c r="C28" s="93"/>
+      <c r="A28" s="87"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
       <c r="D28" s="2" t="s">
         <v>9</v>
       </c>
@@ -2432,9 +2425,9 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="94"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
       <c r="D29" s="2" t="s">
         <v>13</v>
       </c>
@@ -2462,11 +2455,11 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="90" t="s">
+      <c r="A31" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
       <c r="D31" s="2" t="s">
         <v>13</v>
       </c>
@@ -2481,9 +2474,9 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="91"/>
-      <c r="B32" s="93"/>
-      <c r="C32" s="93"/>
+      <c r="A32" s="87"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
       <c r="D32" s="2" t="s">
         <v>13</v>
       </c>
@@ -2498,9 +2491,9 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="94"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="95"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
       <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
@@ -2528,11 +2521,11 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="87" t="s">
+      <c r="A35" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="88"/>
-      <c r="C35" s="88"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="93"/>
       <c r="D35" s="2" t="s">
         <v>13</v>
       </c>
@@ -2547,9 +2540,9 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="87"/>
-      <c r="B36" s="88"/>
-      <c r="C36" s="88"/>
+      <c r="A36" s="92"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="93"/>
       <c r="D36" s="2" t="s">
         <v>9</v>
       </c>
@@ -2564,9 +2557,9 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="87"/>
-      <c r="B37" s="88"/>
-      <c r="C37" s="88"/>
+      <c r="A37" s="92"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
       <c r="D37" s="2" t="s">
         <v>9</v>
       </c>
@@ -2581,9 +2574,9 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="87"/>
-      <c r="B38" s="88"/>
-      <c r="C38" s="88"/>
+      <c r="A38" s="92"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="93"/>
       <c r="D38" s="2" t="s">
         <v>9</v>
       </c>
@@ -2596,9 +2589,9 @@
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="87"/>
-      <c r="B39" s="88"/>
-      <c r="C39" s="88"/>
+      <c r="A39" s="92"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="93"/>
       <c r="D39" s="2" t="s">
         <v>9</v>
       </c>
@@ -2624,11 +2617,11 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
       <c r="D41" s="2" t="s">
         <v>13</v>
       </c>
@@ -2643,9 +2636,9 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="91"/>
-      <c r="B42" s="93"/>
-      <c r="C42" s="93"/>
+      <c r="A42" s="87"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="90"/>
       <c r="D42" s="2" t="s">
         <v>9</v>
       </c>
@@ -2658,9 +2651,9 @@
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="94"/>
-      <c r="B43" s="95"/>
-      <c r="C43" s="95"/>
+      <c r="A43" s="88"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="91"/>
       <c r="D43" s="2" t="s">
         <v>9</v>
       </c>
@@ -2686,11 +2679,11 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="92"/>
-      <c r="C45" s="92"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="89"/>
       <c r="D45" s="2" t="s">
         <v>13</v>
       </c>
@@ -2705,9 +2698,9 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="91"/>
-      <c r="B46" s="93"/>
-      <c r="C46" s="93"/>
+      <c r="A46" s="87"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
       <c r="D46" s="2" t="s">
         <v>13</v>
       </c>
@@ -2722,9 +2715,9 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="91"/>
-      <c r="B47" s="93"/>
-      <c r="C47" s="93"/>
+      <c r="A47" s="87"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="90"/>
       <c r="D47" s="2" t="s">
         <v>9</v>
       </c>
@@ -2737,9 +2730,9 @@
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="91"/>
-      <c r="B48" s="93"/>
-      <c r="C48" s="93"/>
+      <c r="A48" s="87"/>
+      <c r="B48" s="90"/>
+      <c r="C48" s="90"/>
       <c r="D48" s="2" t="s">
         <v>9</v>
       </c>
@@ -2795,11 +2788,11 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="87" t="s">
+      <c r="A52" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="88"/>
-      <c r="C52" s="88"/>
+      <c r="B52" s="93"/>
+      <c r="C52" s="93"/>
       <c r="D52" s="2" t="s">
         <v>13</v>
       </c>
@@ -2814,9 +2807,9 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="87"/>
-      <c r="B53" s="88"/>
-      <c r="C53" s="88"/>
+      <c r="A53" s="92"/>
+      <c r="B53" s="93"/>
+      <c r="C53" s="93"/>
       <c r="D53" s="2" t="s">
         <v>13</v>
       </c>
@@ -2831,9 +2824,9 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="87"/>
-      <c r="B54" s="88"/>
-      <c r="C54" s="88"/>
+      <c r="A54" s="92"/>
+      <c r="B54" s="93"/>
+      <c r="C54" s="93"/>
       <c r="D54" s="2" t="s">
         <v>13</v>
       </c>
@@ -2848,9 +2841,9 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="87"/>
-      <c r="B55" s="88"/>
-      <c r="C55" s="88"/>
+      <c r="A55" s="92"/>
+      <c r="B55" s="93"/>
+      <c r="C55" s="93"/>
       <c r="D55" s="2" t="s">
         <v>9</v>
       </c>
@@ -2863,9 +2856,9 @@
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="87"/>
-      <c r="B56" s="88"/>
-      <c r="C56" s="88"/>
+      <c r="A56" s="92"/>
+      <c r="B56" s="93"/>
+      <c r="C56" s="93"/>
       <c r="D56" s="2" t="s">
         <v>9</v>
       </c>
@@ -2891,11 +2884,11 @@
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="87" t="s">
+      <c r="A58" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="88"/>
-      <c r="C58" s="88"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="93"/>
       <c r="D58" s="2" t="s">
         <v>13</v>
       </c>
@@ -2910,9 +2903,9 @@
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="87"/>
-      <c r="B59" s="88"/>
-      <c r="C59" s="88"/>
+      <c r="A59" s="92"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="93"/>
       <c r="D59" s="2" t="s">
         <v>9</v>
       </c>
@@ -2940,11 +2933,11 @@
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="87" t="s">
+      <c r="A61" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="B61" s="88"/>
-      <c r="C61" s="88"/>
+      <c r="B61" s="93"/>
+      <c r="C61" s="93"/>
       <c r="D61" s="2" t="s">
         <v>13</v>
       </c>
@@ -2959,9 +2952,9 @@
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="87"/>
-      <c r="B62" s="88"/>
-      <c r="C62" s="88"/>
+      <c r="A62" s="92"/>
+      <c r="B62" s="93"/>
+      <c r="C62" s="93"/>
       <c r="D62" s="2" t="s">
         <v>9</v>
       </c>
@@ -2989,11 +2982,11 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="87" t="s">
+      <c r="A64" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="B64" s="89"/>
-      <c r="C64" s="88"/>
+      <c r="B64" s="94"/>
+      <c r="C64" s="93"/>
       <c r="D64" s="2" t="s">
         <v>13</v>
       </c>
@@ -3006,9 +2999,9 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="87"/>
-      <c r="B65" s="89"/>
-      <c r="C65" s="88"/>
+      <c r="A65" s="92"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="93"/>
       <c r="D65" s="2" t="s">
         <v>9</v>
       </c>
@@ -3019,9 +3012,9 @@
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="87"/>
-      <c r="B66" s="89"/>
-      <c r="C66" s="88"/>
+      <c r="A66" s="92"/>
+      <c r="B66" s="94"/>
+      <c r="C66" s="93"/>
       <c r="D66" s="2" t="s">
         <v>9</v>
       </c>
@@ -3047,11 +3040,11 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="87" t="s">
+      <c r="A68" s="92" t="s">
         <v>112</v>
       </c>
-      <c r="B68" s="88"/>
-      <c r="C68" s="88"/>
+      <c r="B68" s="93"/>
+      <c r="C68" s="93"/>
       <c r="D68" s="2" t="s">
         <v>13</v>
       </c>
@@ -3066,9 +3059,9 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="87"/>
-      <c r="B69" s="88"/>
-      <c r="C69" s="88"/>
+      <c r="A69" s="92"/>
+      <c r="B69" s="93"/>
+      <c r="C69" s="93"/>
       <c r="D69" s="2" t="s">
         <v>9</v>
       </c>
@@ -3081,9 +3074,9 @@
       <c r="G69" s="4"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="87"/>
-      <c r="B70" s="88"/>
-      <c r="C70" s="88"/>
+      <c r="A70" s="92"/>
+      <c r="B70" s="93"/>
+      <c r="C70" s="93"/>
       <c r="D70" s="2" t="s">
         <v>9</v>
       </c>
@@ -3096,9 +3089,9 @@
       <c r="G70" s="4"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="87"/>
-      <c r="B71" s="88"/>
-      <c r="C71" s="88"/>
+      <c r="A71" s="92"/>
+      <c r="B71" s="93"/>
+      <c r="C71" s="93"/>
       <c r="D71" s="2" t="s">
         <v>9</v>
       </c>
@@ -3124,11 +3117,11 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="87" t="s">
+      <c r="A73" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="88"/>
-      <c r="C73" s="88"/>
+      <c r="B73" s="93"/>
+      <c r="C73" s="93"/>
       <c r="D73" s="2" t="s">
         <v>13</v>
       </c>
@@ -3143,9 +3136,9 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="87"/>
-      <c r="B74" s="88"/>
-      <c r="C74" s="88"/>
+      <c r="A74" s="92"/>
+      <c r="B74" s="93"/>
+      <c r="C74" s="93"/>
       <c r="D74" s="2" t="s">
         <v>9</v>
       </c>
@@ -3158,9 +3151,9 @@
       <c r="G74" s="4"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="87"/>
-      <c r="B75" s="88"/>
-      <c r="C75" s="88"/>
+      <c r="A75" s="92"/>
+      <c r="B75" s="93"/>
+      <c r="C75" s="93"/>
       <c r="D75" s="2" t="s">
         <v>9</v>
       </c>
@@ -3173,9 +3166,9 @@
       <c r="G75" s="4"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="87"/>
-      <c r="B76" s="88"/>
-      <c r="C76" s="88"/>
+      <c r="A76" s="92"/>
+      <c r="B76" s="93"/>
+      <c r="C76" s="93"/>
       <c r="D76" s="2" t="s">
         <v>9</v>
       </c>
@@ -3201,11 +3194,11 @@
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="87" t="s">
+      <c r="A78" s="92" t="s">
         <v>129</v>
       </c>
-      <c r="B78" s="88"/>
-      <c r="C78" s="88"/>
+      <c r="B78" s="93"/>
+      <c r="C78" s="93"/>
       <c r="D78" s="2" t="s">
         <v>13</v>
       </c>
@@ -3220,9 +3213,9 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="87"/>
-      <c r="B79" s="88"/>
-      <c r="C79" s="88"/>
+      <c r="A79" s="92"/>
+      <c r="B79" s="93"/>
+      <c r="C79" s="93"/>
       <c r="D79" s="2" t="s">
         <v>9</v>
       </c>
@@ -3237,9 +3230,9 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="105" customHeight="1">
-      <c r="A80" s="87"/>
-      <c r="B80" s="88"/>
-      <c r="C80" s="88"/>
+      <c r="A80" s="92"/>
+      <c r="B80" s="93"/>
+      <c r="C80" s="93"/>
       <c r="D80" s="2" t="s">
         <v>9</v>
       </c>
@@ -3265,11 +3258,11 @@
       </c>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="87" t="s">
+      <c r="A82" s="92" t="s">
         <v>135</v>
       </c>
-      <c r="B82" s="88"/>
-      <c r="C82" s="88" t="s">
+      <c r="B82" s="93"/>
+      <c r="C82" s="93" t="s">
         <v>136</v>
       </c>
       <c r="D82" s="2" t="s">
@@ -3286,9 +3279,9 @@
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="87"/>
-      <c r="B83" s="88"/>
-      <c r="C83" s="88"/>
+      <c r="A83" s="92"/>
+      <c r="B83" s="93"/>
+      <c r="C83" s="93"/>
       <c r="D83" s="2" t="s">
         <v>9</v>
       </c>
@@ -3301,9 +3294,9 @@
       <c r="G83" s="4"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="87"/>
-      <c r="B84" s="88"/>
-      <c r="C84" s="88"/>
+      <c r="A84" s="92"/>
+      <c r="B84" s="93"/>
+      <c r="C84" s="93"/>
       <c r="D84" s="2" t="s">
         <v>9</v>
       </c>
@@ -3329,14 +3322,14 @@
       </c>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="87" t="s">
+      <c r="A86" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="B86" s="88"/>
-      <c r="C86" s="87" t="s">
+      <c r="B86" s="93"/>
+      <c r="C86" s="92" t="s">
         <v>142</v>
       </c>
-      <c r="D86" s="84" t="s">
+      <c r="D86" s="95" t="s">
         <v>9</v>
       </c>
       <c r="E86" s="33" t="s">
@@ -3348,10 +3341,10 @@
       <c r="G86" s="4"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="87"/>
-      <c r="B87" s="88"/>
-      <c r="C87" s="87"/>
-      <c r="D87" s="85"/>
+      <c r="A87" s="92"/>
+      <c r="B87" s="93"/>
+      <c r="C87" s="92"/>
+      <c r="D87" s="96"/>
       <c r="E87" s="32" t="s">
         <v>145</v>
       </c>
@@ -3361,10 +3354,10 @@
       <c r="G87" s="4"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="87"/>
-      <c r="B88" s="88"/>
-      <c r="C88" s="87"/>
-      <c r="D88" s="86"/>
+      <c r="A88" s="92"/>
+      <c r="B88" s="93"/>
+      <c r="C88" s="92"/>
+      <c r="D88" s="97"/>
       <c r="E88" s="32" t="s">
         <v>146</v>
       </c>
@@ -3374,9 +3367,9 @@
       <c r="G88" s="4"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="87"/>
-      <c r="B89" s="88"/>
-      <c r="C89" s="87"/>
+      <c r="A89" s="92"/>
+      <c r="B89" s="93"/>
+      <c r="C89" s="92"/>
       <c r="D89" s="2" t="s">
         <v>9</v>
       </c>
@@ -3402,11 +3395,11 @@
       </c>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="87" t="s">
+      <c r="A91" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="B91" s="88"/>
-      <c r="C91" s="87" t="s">
+      <c r="B91" s="93"/>
+      <c r="C91" s="92" t="s">
         <v>151</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -3421,9 +3414,9 @@
       <c r="G91" s="4"/>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="87"/>
-      <c r="B92" s="87"/>
-      <c r="C92" s="87"/>
+      <c r="A92" s="92"/>
+      <c r="B92" s="92"/>
+      <c r="C92" s="92"/>
       <c r="D92" s="2" t="s">
         <v>9</v>
       </c>
@@ -3438,9 +3431,9 @@
       </c>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="87"/>
-      <c r="B93" s="87"/>
-      <c r="C93" s="87"/>
+      <c r="A93" s="92"/>
+      <c r="B93" s="92"/>
+      <c r="C93" s="92"/>
       <c r="D93" s="2" t="s">
         <v>9</v>
       </c>
@@ -3453,9 +3446,9 @@
       <c r="G93" s="4"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="87"/>
-      <c r="B94" s="87"/>
-      <c r="C94" s="87"/>
+      <c r="A94" s="92"/>
+      <c r="B94" s="92"/>
+      <c r="C94" s="92"/>
       <c r="D94" s="2" t="s">
         <v>9</v>
       </c>
@@ -3495,56 +3488,6 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="C35:C39"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
     <mergeCell ref="D86:D88"/>
     <mergeCell ref="A91:A94"/>
     <mergeCell ref="B91:B94"/>
@@ -3555,6 +3498,56 @@
     <mergeCell ref="A86:A89"/>
     <mergeCell ref="B86:B89"/>
     <mergeCell ref="C86:C89"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{A2F3A9F3-D399-4DBA-B2A6-837F2CB9A7BA}"/>
@@ -3639,7 +3632,7 @@
   </sheetPr>
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3648,7 +3641,7 @@
     <col min="1" max="1" width="13.28515625" style="75" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="75" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="75" customWidth="1"/>
-    <col min="4" max="4" width="65.5703125" style="75" customWidth="1"/>
+    <col min="4" max="4" width="93.140625" style="75" customWidth="1"/>
     <col min="5" max="5" width="90" style="75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" style="75" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="75"/>
@@ -3685,10 +3678,10 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="103">
+      <c r="B3" s="102">
         <v>45190</v>
       </c>
       <c r="C3" s="49" t="s">
@@ -3705,8 +3698,8 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="102"/>
-      <c r="B4" s="102"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="49" t="s">
         <v>9</v>
       </c>
@@ -3721,40 +3714,40 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="102"/>
-      <c r="B5" s="102"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" t="s">
         <v>162</v>
       </c>
       <c r="E5" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="F5" s="52" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="102"/>
-      <c r="B6" s="102"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="E6" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="52" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="102"/>
-      <c r="B7" s="102"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="49" t="s">
         <v>9</v>
       </c>
@@ -3765,12 +3758,12 @@
         <v>17</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="49" t="s">
         <v>9</v>
       </c>
@@ -3781,7 +3774,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3801,48 +3794,48 @@
         <v>19</v>
       </c>
       <c r="F9" s="58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="105" t="s">
+      <c r="A10" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="106">
+      <c r="B10" s="105">
         <v>45191</v>
       </c>
       <c r="C10" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="E10" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="F10" s="59" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="105"/>
-      <c r="B11" s="105"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="104"/>
       <c r="C11" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="76" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11" s="59" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="105"/>
-      <c r="B12" s="105"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="49" t="s">
         <v>9</v>
       </c>
@@ -3857,8 +3850,8 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="105"/>
-      <c r="B13" s="105"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="104"/>
       <c r="C13" s="49" t="s">
         <v>9</v>
       </c>
@@ -3873,8 +3866,8 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="105"/>
-      <c r="B14" s="105"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="49" t="s">
         <v>9</v>
       </c>
@@ -3889,35 +3882,35 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="105"/>
-      <c r="B15" s="105"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="49" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="E15" s="62" t="s">
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="E16" s="63" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="105"/>
-      <c r="B16" s="105"/>
-      <c r="C16" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="76" t="s">
+      <c r="F16" s="52" t="s">
         <v>180</v>
-      </c>
-      <c r="E16" s="63" t="s">
-        <v>181</v>
-      </c>
-      <c r="F16" s="52" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3937,48 +3930,48 @@
         <v>28</v>
       </c>
       <c r="F17" s="58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="102" t="s">
+      <c r="A18" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="103">
+      <c r="B18" s="102">
         <v>45192</v>
       </c>
       <c r="C18" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="E18" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="F18" s="59" t="s">
-        <v>186</v>
-      </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="102"/>
-      <c r="B19" s="102"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="101"/>
       <c r="C19" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="F19" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="E19" s="49" t="s">
-        <v>188</v>
-      </c>
-      <c r="F19" s="59" t="s">
-        <v>189</v>
-      </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="102"/>
-      <c r="B20" s="102"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="101"/>
       <c r="C20" s="49" t="s">
         <v>9</v>
       </c>
@@ -3993,8 +3986,8 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="102"/>
-      <c r="B21" s="102"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="101"/>
       <c r="C21" s="49" t="s">
         <v>9</v>
       </c>
@@ -4009,8 +4002,8 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="102"/>
-      <c r="B22" s="102"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="101"/>
       <c r="C22" s="49" t="s">
         <v>9</v>
       </c>
@@ -4025,8 +4018,8 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="104"/>
-      <c r="B23" s="104"/>
+      <c r="A23" s="103"/>
+      <c r="B23" s="103"/>
       <c r="C23" s="49" t="s">
         <v>9</v>
       </c>
@@ -4057,32 +4050,32 @@
         <v>37</v>
       </c>
       <c r="F24" s="58" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="104" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="105">
+        <v>45194</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" s="63" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="105" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="106">
-        <v>45194</v>
-      </c>
-      <c r="C25" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="76" t="s">
+      <c r="F25" s="65" t="s">
         <v>191</v>
       </c>
-      <c r="E25" s="63" t="s">
-        <v>192</v>
-      </c>
-      <c r="F25" s="65" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="105"/>
-      <c r="B26" s="105"/>
+      <c r="A26" s="104"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="49" t="s">
         <v>9</v>
       </c>
@@ -4097,8 +4090,8 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="105"/>
-      <c r="B27" s="105"/>
+      <c r="A27" s="104"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="49" t="s">
         <v>9</v>
       </c>
@@ -4113,8 +4106,8 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="105"/>
-      <c r="B28" s="105"/>
+      <c r="A28" s="104"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="49" t="s">
         <v>9</v>
       </c>
@@ -4129,8 +4122,8 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="105"/>
-      <c r="B29" s="105"/>
+      <c r="A29" s="104"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="49" t="s">
         <v>9</v>
       </c>
@@ -4145,19 +4138,19 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="105"/>
-      <c r="B30" s="105"/>
+      <c r="A30" s="104"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="F30" s="52" t="s">
         <v>194</v>
-      </c>
-      <c r="E30" s="49" t="s">
-        <v>195</v>
-      </c>
-      <c r="F30" s="52" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4177,14 +4170,14 @@
         <v>46</v>
       </c>
       <c r="F31" s="58" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="102" t="s">
+      <c r="A32" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="103">
+      <c r="B32" s="102">
         <v>45195</v>
       </c>
       <c r="C32" s="49" t="s">
@@ -4197,39 +4190,39 @@
         <v>42</v>
       </c>
       <c r="F32" s="52" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="102"/>
-      <c r="B33" s="102"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="F33" s="52" t="s">
         <v>198</v>
       </c>
-      <c r="E33" s="49" t="s">
-        <v>199</v>
-      </c>
-      <c r="F33" s="52" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="102"/>
-      <c r="B34" s="102"/>
+      <c r="A34" s="101"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="76" t="s">
+        <v>199</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="52" t="s">
         <v>201</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>202</v>
-      </c>
-      <c r="F34" s="52" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4249,48 +4242,48 @@
         <v>53</v>
       </c>
       <c r="F35" s="58" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="103">
+      <c r="B36" s="102">
         <v>45196</v>
       </c>
       <c r="C36" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="F36" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="E36" s="49" t="s">
-        <v>206</v>
-      </c>
-      <c r="F36" s="52" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="102"/>
-      <c r="B37" s="102"/>
+      <c r="A37" s="101"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="76" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="52" t="s">
         <v>208</v>
       </c>
-      <c r="E37" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="F37" s="52" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="104"/>
-      <c r="B38" s="104"/>
+      <c r="A38" s="103"/>
+      <c r="B38" s="103"/>
       <c r="C38" s="49" t="s">
         <v>9</v>
       </c>
@@ -4301,7 +4294,7 @@
         <v>42</v>
       </c>
       <c r="F38" s="52" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -4321,48 +4314,48 @@
         <v>59</v>
       </c>
       <c r="F39" s="58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="102" t="s">
+      <c r="A40" s="101" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="103">
+      <c r="B40" s="102">
         <v>45197</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="76" t="s">
+        <v>211</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="F40" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="E40" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="F40" s="52" t="s">
-        <v>215</v>
-      </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="102"/>
-      <c r="B41" s="102"/>
+      <c r="A41" s="101"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="76" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E41" s="49" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F41" s="52" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="102"/>
-      <c r="B42" s="102"/>
+      <c r="A42" s="101"/>
+      <c r="B42" s="101"/>
       <c r="C42" s="49" t="s">
         <v>9</v>
       </c>
@@ -4373,12 +4366,12 @@
         <v>64</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="102"/>
-      <c r="B43" s="102"/>
+      <c r="A43" s="101"/>
+      <c r="B43" s="101"/>
       <c r="C43" s="49" t="s">
         <v>9</v>
       </c>
@@ -4389,12 +4382,12 @@
         <v>64</v>
       </c>
       <c r="F43" s="52" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="102"/>
-      <c r="B44" s="102"/>
+      <c r="A44" s="101"/>
+      <c r="B44" s="101"/>
       <c r="C44" s="49" t="s">
         <v>9</v>
       </c>
@@ -4409,8 +4402,8 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="107"/>
-      <c r="B45" s="107"/>
+      <c r="A45" s="106"/>
+      <c r="B45" s="106"/>
       <c r="C45" s="49" t="s">
         <v>9</v>
       </c>
@@ -4441,48 +4434,48 @@
         <v>68</v>
       </c>
       <c r="F46" s="58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="102" t="s">
+      <c r="A47" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="103">
+      <c r="B47" s="102">
         <v>45198</v>
       </c>
       <c r="C47" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="E47" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="F47" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="E47" s="49" t="s">
-        <v>221</v>
-      </c>
-      <c r="F47" s="52" t="s">
-        <v>222</v>
-      </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="102"/>
-      <c r="B48" s="102"/>
+      <c r="A48" s="101"/>
+      <c r="B48" s="101"/>
       <c r="C48" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="76" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E48" s="49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F48" s="52" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="102"/>
-      <c r="B49" s="102"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
       <c r="C49" s="49" t="s">
         <v>9</v>
       </c>
@@ -4497,8 +4490,8 @@
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="104"/>
-      <c r="B50" s="104"/>
+      <c r="A50" s="103"/>
+      <c r="B50" s="103"/>
       <c r="C50" s="49" t="s">
         <v>9</v>
       </c>
@@ -4529,48 +4522,48 @@
         <v>74</v>
       </c>
       <c r="F51" s="58" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="102" t="s">
+      <c r="A52" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="B52" s="103">
+      <c r="B52" s="102">
         <v>45199</v>
       </c>
       <c r="C52" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="76" t="s">
+        <v>224</v>
+      </c>
+      <c r="E52" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="F52" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="E52" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="F52" s="52" t="s">
-        <v>228</v>
-      </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="102"/>
-      <c r="B53" s="102"/>
+      <c r="A53" s="101"/>
+      <c r="B53" s="101"/>
       <c r="C53" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="76" t="s">
+        <v>227</v>
+      </c>
+      <c r="E53" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="F53" s="52" t="s">
         <v>229</v>
       </c>
-      <c r="E53" s="49" t="s">
-        <v>230</v>
-      </c>
-      <c r="F53" s="52" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="102"/>
-      <c r="B54" s="102"/>
+      <c r="A54" s="101"/>
+      <c r="B54" s="101"/>
       <c r="C54" s="49" t="s">
         <v>9</v>
       </c>
@@ -4585,8 +4578,8 @@
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="102"/>
-      <c r="B55" s="102"/>
+      <c r="A55" s="101"/>
+      <c r="B55" s="101"/>
       <c r="C55" s="49" t="s">
         <v>9</v>
       </c>
@@ -4617,43 +4610,43 @@
         <v>83</v>
       </c>
       <c r="F56" s="58" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="101" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="107">
+        <v>45202</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="E57" s="50" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="102" t="s">
-        <v>84</v>
-      </c>
-      <c r="B57" s="108">
-        <v>45202</v>
-      </c>
-      <c r="C57" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="76" t="s">
+      <c r="F57" s="52" t="s">
         <v>233</v>
       </c>
-      <c r="E57" s="50" t="s">
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="106"/>
+      <c r="B58" s="108"/>
+      <c r="C58" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="F57" s="52" t="s">
+      <c r="E58" s="50" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="107"/>
-      <c r="B58" s="109"/>
-      <c r="C58" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="80" t="s">
+      <c r="F58" s="52" t="s">
         <v>236</v>
-      </c>
-      <c r="E58" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F58" s="52" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -4673,64 +4666,64 @@
         <v>86</v>
       </c>
       <c r="F59" s="58" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="102" t="s">
+      <c r="A60" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="B60" s="103">
+      <c r="B60" s="102">
         <v>45203</v>
       </c>
       <c r="C60" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="76" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E60" s="49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F60" s="52" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="102"/>
-      <c r="B61" s="102"/>
+      <c r="A61" s="101"/>
+      <c r="B61" s="101"/>
       <c r="C61" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D61" s="76" t="s">
+        <v>240</v>
+      </c>
+      <c r="E61" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="F61" s="52" t="s">
         <v>242</v>
       </c>
-      <c r="E61" s="49" t="s">
-        <v>243</v>
-      </c>
-      <c r="F61" s="52" t="s">
-        <v>244</v>
-      </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="102"/>
-      <c r="B62" s="102"/>
+      <c r="A62" s="101"/>
+      <c r="B62" s="101"/>
       <c r="C62" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D62" s="76" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E62" s="49" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F62" s="52" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="102"/>
-      <c r="B63" s="102"/>
+      <c r="A63" s="101"/>
+      <c r="B63" s="101"/>
       <c r="C63" s="49" t="s">
         <v>9</v>
       </c>
@@ -4745,8 +4738,8 @@
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="107"/>
-      <c r="B64" s="107"/>
+      <c r="A64" s="106"/>
+      <c r="B64" s="106"/>
       <c r="C64" s="49" t="s">
         <v>9</v>
       </c>
@@ -4777,48 +4770,48 @@
         <v>96</v>
       </c>
       <c r="F65" s="58" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="102" t="s">
+      <c r="A66" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="103">
+      <c r="B66" s="102">
         <v>45204</v>
       </c>
       <c r="C66" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="76" t="s">
+        <v>246</v>
+      </c>
+      <c r="E66" s="49" t="s">
+        <v>247</v>
+      </c>
+      <c r="F66" s="52" t="s">
         <v>248</v>
       </c>
-      <c r="E66" s="49" t="s">
-        <v>249</v>
-      </c>
-      <c r="F66" s="52" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="102"/>
-      <c r="B67" s="102"/>
+      <c r="A67" s="101"/>
+      <c r="B67" s="101"/>
       <c r="C67" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D67" s="76" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E67" s="49" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F67" s="52" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="107"/>
-      <c r="B68" s="107"/>
+      <c r="A68" s="106"/>
+      <c r="B68" s="106"/>
       <c r="C68" s="49" t="s">
         <v>9</v>
       </c>
@@ -4829,7 +4822,7 @@
         <v>81</v>
       </c>
       <c r="F68" s="52" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4849,75 +4842,75 @@
         <v>101</v>
       </c>
       <c r="F69" s="58" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="102" t="s">
+      <c r="A70" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="B70" s="103">
+      <c r="B70" s="102">
         <v>45205</v>
       </c>
       <c r="C70" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D70" s="76" t="s">
+        <v>253</v>
+      </c>
+      <c r="E70" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="F70" s="52" t="s">
         <v>255</v>
       </c>
-      <c r="E70" s="49" t="s">
-        <v>256</v>
-      </c>
-      <c r="F70" s="52" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="102"/>
-      <c r="B71" s="102"/>
+      <c r="A71" s="101"/>
+      <c r="B71" s="101"/>
       <c r="C71" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D71" s="76" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E71" s="49" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="102"/>
-      <c r="B72" s="102"/>
+      <c r="A72" s="101"/>
+      <c r="B72" s="101"/>
       <c r="C72" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="76" t="s">
+        <v>258</v>
+      </c>
+      <c r="E72" s="49" t="s">
+        <v>259</v>
+      </c>
+      <c r="F72" s="52" t="s">
         <v>260</v>
       </c>
-      <c r="E72" s="49" t="s">
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="106"/>
+      <c r="B73" s="106"/>
+      <c r="C73" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="76" t="s">
         <v>261</v>
       </c>
-      <c r="F72" s="52" t="s">
+      <c r="E73" s="49" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="107"/>
-      <c r="B73" s="107"/>
-      <c r="C73" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="76" t="s">
+      <c r="F73" s="52" t="s">
         <v>263</v>
-      </c>
-      <c r="E73" s="49" t="s">
-        <v>264</v>
-      </c>
-      <c r="F73" s="52" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4931,13 +4924,13 @@
         <v>9</v>
       </c>
       <c r="D74" s="80" t="s">
+        <v>264</v>
+      </c>
+      <c r="E74" s="49" t="s">
+        <v>265</v>
+      </c>
+      <c r="F74" s="52" t="s">
         <v>266</v>
-      </c>
-      <c r="E74" s="49" t="s">
-        <v>267</v>
-      </c>
-      <c r="F74" s="52" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -4957,48 +4950,48 @@
         <v>106</v>
       </c>
       <c r="F75" s="58" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="102" t="s">
+      <c r="A76" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="B76" s="110">
+      <c r="B76" s="109">
         <v>45206</v>
       </c>
       <c r="C76" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D76" s="76" t="s">
+        <v>268</v>
+      </c>
+      <c r="E76" s="49" t="s">
+        <v>269</v>
+      </c>
+      <c r="F76" s="52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="101"/>
+      <c r="B77" s="110"/>
+      <c r="C77" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="D77" s="76" t="s">
         <v>270</v>
       </c>
-      <c r="E76" s="49" t="s">
+      <c r="E77" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="F76" s="52" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="102"/>
-      <c r="B77" s="111"/>
-      <c r="C77" s="49" t="s">
-        <v>161</v>
-      </c>
-      <c r="D77" s="76" t="s">
-        <v>272</v>
-      </c>
-      <c r="E77" s="49" t="s">
-        <v>273</v>
-      </c>
       <c r="F77" s="52" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="102"/>
-      <c r="B78" s="111"/>
+      <c r="A78" s="101"/>
+      <c r="B78" s="110"/>
       <c r="C78" s="49" t="s">
         <v>9</v>
       </c>
@@ -5013,19 +5006,19 @@
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="107"/>
-      <c r="B79" s="112"/>
+      <c r="A79" s="106"/>
+      <c r="B79" s="111"/>
       <c r="C79" s="49" t="s">
         <v>9</v>
       </c>
       <c r="D79" s="76" t="s">
+        <v>272</v>
+      </c>
+      <c r="E79" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="F79" s="52" t="s">
         <v>274</v>
-      </c>
-      <c r="E79" s="50" t="s">
-        <v>275</v>
-      </c>
-      <c r="F79" s="52" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -5045,12 +5038,12 @@
         <v>111</v>
       </c>
       <c r="F80" s="58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="68" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B81" s="83">
         <v>45208</v>
@@ -5059,13 +5052,13 @@
         <v>9</v>
       </c>
       <c r="D81" s="76" t="s">
+        <v>276</v>
+      </c>
+      <c r="E81" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="F81" s="52" t="s">
         <v>278</v>
-      </c>
-      <c r="E81" s="50" t="s">
-        <v>279</v>
-      </c>
-      <c r="F81" s="52" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -5082,35 +5075,35 @@
         <v>161</v>
       </c>
       <c r="E82" s="64" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F82" s="58" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="102" t="s">
+      <c r="A83" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="B83" s="103">
+      <c r="B83" s="102">
         <v>45209</v>
       </c>
       <c r="C83" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D83" s="76" t="s">
+        <v>281</v>
+      </c>
+      <c r="E83" s="49" t="s">
+        <v>282</v>
+      </c>
+      <c r="F83" s="52" t="s">
         <v>283</v>
       </c>
-      <c r="E83" s="49" t="s">
-        <v>284</v>
-      </c>
-      <c r="F83" s="52" t="s">
-        <v>285</v>
-      </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="102"/>
-      <c r="B84" s="102"/>
+      <c r="A84" s="101"/>
+      <c r="B84" s="101"/>
       <c r="C84" s="49" t="s">
         <v>9</v>
       </c>
@@ -5125,8 +5118,8 @@
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="102"/>
-      <c r="B85" s="102"/>
+      <c r="A85" s="101"/>
+      <c r="B85" s="101"/>
       <c r="C85" s="49" t="s">
         <v>9</v>
       </c>
@@ -5141,8 +5134,8 @@
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="107"/>
-      <c r="B86" s="107"/>
+      <c r="A86" s="106"/>
+      <c r="B86" s="106"/>
       <c r="C86" s="49" t="s">
         <v>9</v>
       </c>
@@ -5173,48 +5166,48 @@
         <v>134</v>
       </c>
       <c r="F87" s="58" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="102" t="s">
+      <c r="A88" s="101" t="s">
         <v>135</v>
       </c>
-      <c r="B88" s="103">
+      <c r="B88" s="102">
         <v>45210</v>
       </c>
       <c r="C88" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="76" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E88" s="49" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F88" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="102"/>
-      <c r="B89" s="102"/>
+      <c r="A89" s="101"/>
+      <c r="B89" s="101"/>
       <c r="C89" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D89" s="76" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E89" s="49" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F89" s="50" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="102"/>
-      <c r="B90" s="102"/>
+      <c r="A90" s="101"/>
+      <c r="B90" s="101"/>
       <c r="C90" s="49" t="s">
         <v>9</v>
       </c>
@@ -5229,8 +5222,8 @@
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="102"/>
-      <c r="B91" s="102"/>
+      <c r="A91" s="101"/>
+      <c r="B91" s="101"/>
       <c r="C91" s="49" t="s">
         <v>9</v>
       </c>
@@ -5245,8 +5238,8 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="107"/>
-      <c r="B92" s="107"/>
+      <c r="A92" s="106"/>
+      <c r="B92" s="106"/>
       <c r="C92" s="49" t="s">
         <v>9</v>
       </c>
@@ -5277,32 +5270,32 @@
         <v>140</v>
       </c>
       <c r="F93" s="58" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="102">
+        <v>45211</v>
+      </c>
+      <c r="C94" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" s="76" t="s">
+        <v>290</v>
+      </c>
+      <c r="E94" s="49" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="102" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="103">
-        <v>45211</v>
-      </c>
-      <c r="C94" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D94" s="76" t="s">
-        <v>292</v>
-      </c>
-      <c r="E94" s="49" t="s">
-        <v>293</v>
-      </c>
       <c r="F94" s="52" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="76.5">
-      <c r="A95" s="107"/>
-      <c r="B95" s="107"/>
+      <c r="A95" s="106"/>
+      <c r="B95" s="106"/>
       <c r="C95" s="49" t="s">
         <v>9</v>
       </c>
@@ -5333,32 +5326,32 @@
         <v>149</v>
       </c>
       <c r="F96" s="58" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="102" t="s">
+      <c r="A97" s="101" t="s">
         <v>150</v>
       </c>
-      <c r="B97" s="103">
+      <c r="B97" s="102">
         <v>45212</v>
       </c>
       <c r="C97" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D97" s="76" t="s">
+        <v>292</v>
+      </c>
+      <c r="E97" s="49" t="s">
+        <v>293</v>
+      </c>
+      <c r="F97" s="52" t="s">
         <v>294</v>
       </c>
-      <c r="E97" s="49" t="s">
-        <v>295</v>
-      </c>
-      <c r="F97" s="52" t="s">
-        <v>296</v>
-      </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="102"/>
-      <c r="B98" s="102"/>
+      <c r="A98" s="101"/>
+      <c r="B98" s="101"/>
       <c r="C98" s="49" t="s">
         <v>9</v>
       </c>
@@ -5373,19 +5366,19 @@
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="107"/>
-      <c r="B99" s="107"/>
+      <c r="A99" s="106"/>
+      <c r="B99" s="106"/>
       <c r="C99" s="49" t="s">
         <v>9</v>
       </c>
       <c r="D99" s="76" t="s">
+        <v>295</v>
+      </c>
+      <c r="E99" s="49" t="s">
+        <v>296</v>
+      </c>
+      <c r="F99" s="52" t="s">
         <v>297</v>
-      </c>
-      <c r="E99" s="49" t="s">
-        <v>298</v>
-      </c>
-      <c r="F99" s="52" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -5405,17 +5398,17 @@
         <v>157</v>
       </c>
       <c r="F100" s="58" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="102" t="s">
-        <v>301</v>
-      </c>
-      <c r="B101" s="103">
+      <c r="A101" s="101" t="s">
+        <v>299</v>
+      </c>
+      <c r="B101" s="102">
         <v>45213</v>
       </c>
-      <c r="C101" s="102" t="s">
+      <c r="C101" s="101" t="s">
         <v>9</v>
       </c>
       <c r="D101" s="49" t="s">
@@ -5429,9 +5422,9 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="102"/>
-      <c r="B102" s="102"/>
-      <c r="C102" s="102"/>
+      <c r="A102" s="101"/>
+      <c r="B102" s="101"/>
+      <c r="C102" s="101"/>
       <c r="D102" s="76" t="s">
         <v>145</v>
       </c>
@@ -5443,9 +5436,9 @@
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="102"/>
-      <c r="B103" s="102"/>
-      <c r="C103" s="104"/>
+      <c r="A103" s="101"/>
+      <c r="B103" s="101"/>
+      <c r="C103" s="103"/>
       <c r="D103" s="76" t="s">
         <v>146</v>
       </c>
@@ -5457,8 +5450,8 @@
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="107"/>
-      <c r="B104" s="107"/>
+      <c r="A104" s="106"/>
+      <c r="B104" s="106"/>
       <c r="C104" s="49" t="s">
         <v>9</v>
       </c>
@@ -5486,17 +5479,17 @@
         <v>161</v>
       </c>
       <c r="E105" s="64" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F105" s="58" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="102" t="s">
-        <v>303</v>
-      </c>
-      <c r="B106" s="103">
+      <c r="A106" s="101" t="s">
+        <v>301</v>
+      </c>
+      <c r="B106" s="102">
         <v>45215</v>
       </c>
       <c r="C106" s="49" t="s">
@@ -5513,24 +5506,24 @@
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="102"/>
-      <c r="B107" s="102"/>
+      <c r="A107" s="101"/>
+      <c r="B107" s="101"/>
       <c r="C107" s="49" t="s">
         <v>9</v>
       </c>
       <c r="D107" s="76" t="s">
+        <v>302</v>
+      </c>
+      <c r="E107" s="49" t="s">
+        <v>303</v>
+      </c>
+      <c r="F107" s="52" t="s">
         <v>304</v>
       </c>
-      <c r="E107" s="49" t="s">
-        <v>305</v>
-      </c>
-      <c r="F107" s="52" t="s">
-        <v>306</v>
-      </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="102"/>
-      <c r="B108" s="102"/>
+      <c r="A108" s="101"/>
+      <c r="B108" s="101"/>
       <c r="C108" s="49" t="s">
         <v>9</v>
       </c>
@@ -5545,8 +5538,8 @@
       </c>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="107"/>
-      <c r="B109" s="107"/>
+      <c r="A109" s="106"/>
+      <c r="B109" s="106"/>
       <c r="C109" s="49" t="s">
         <v>9</v>
       </c>
@@ -5574,10 +5567,10 @@
         <v>161</v>
       </c>
       <c r="E110" s="64" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F110" s="58" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -5602,6 +5595,41 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A101:A104"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="A88:A92"/>
+    <mergeCell ref="B88:B92"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="A40:A45"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
     <mergeCell ref="A18:A23"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="A1:F1"/>
@@ -5609,41 +5637,6 @@
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="B10:B16"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A40:A45"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="B83:B86"/>
-    <mergeCell ref="A88:A92"/>
-    <mergeCell ref="B88:B92"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="A101:A104"/>
-    <mergeCell ref="B101:B104"/>
-    <mergeCell ref="C101:C103"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="B106:B109"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{0799226B-874C-4709-8B50-7D16C23CB9CA}"/>

</xml_diff>